<commit_message>
redbus count number of buses
</commit_message>
<xml_diff>
--- a/com.pathnxt.test/src/test/resources/TestData.xlsx
+++ b/com.pathnxt.test/src/test/resources/TestData.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16275" windowHeight="4275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="irctc" sheetId="1" r:id="rId1"/>
+    <sheet name="redbus" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:P12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>from</t>
   </si>
@@ -41,6 +43,12 @@
   </si>
   <si>
     <t>LOWER</t>
+  </si>
+  <si>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>bengaluru</t>
   </si>
 </sst>
 </file>
@@ -391,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,4 +443,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Fetched the data from the excel sheet and done some optimization
</commit_message>
<xml_diff>
--- a/com.pathnxt.test/src/test/resources/TestData.xlsx
+++ b/com.pathnxt.test/src/test/resources/TestData.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16275" windowHeight="4275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="4275" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="irctc" sheetId="1" r:id="rId1"/>
     <sheet name="redbus" sheetId="2" r:id="rId2"/>
+    <sheet name="window" sheetId="3" r:id="rId3"/>
+    <sheet name="tab" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P12"/>
+  <oleSize ref="A1:I12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>from</t>
   </si>
@@ -49,6 +51,72 @@
   </si>
   <si>
     <t>bengaluru</t>
+  </si>
+  <si>
+    <t>child window title</t>
+  </si>
+  <si>
+    <t>parent window title</t>
+  </si>
+  <si>
+    <t>child window txtfield</t>
+  </si>
+  <si>
+    <t>parent window txtfield</t>
+  </si>
+  <si>
+    <t>child txtxfield</t>
+  </si>
+  <si>
+    <t>parent txtfield</t>
+  </si>
+  <si>
+    <t>confirmation message</t>
+  </si>
+  <si>
+    <t>test case passed</t>
+  </si>
+  <si>
+    <t>url number</t>
+  </si>
+  <si>
+    <t>url3</t>
+  </si>
+  <si>
+    <t>Window Handles Practice - H Y R Tutorials</t>
+  </si>
+  <si>
+    <t>Basic Controls - H Y R Tutorials</t>
+  </si>
+  <si>
+    <t>parent tab</t>
+  </si>
+  <si>
+    <t>child tab</t>
+  </si>
+  <si>
+    <t>messgae</t>
+  </si>
+  <si>
+    <t>alert message</t>
+  </si>
+  <si>
+    <t>AlertsDemo - H Y R Tutorials</t>
+  </si>
+  <si>
+    <t>I am an alert box!</t>
+  </si>
+  <si>
+    <t>XPath Practice - H Y R Tutorials</t>
+  </si>
+  <si>
+    <t>child txtxfield2</t>
+  </si>
+  <si>
+    <t>This is parent tab</t>
+  </si>
+  <si>
+    <t>Hello!</t>
   </si>
 </sst>
 </file>
@@ -449,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -480,4 +548,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added takescreenshot,robot class and hard assert
</commit_message>
<xml_diff>
--- a/com.pathnxt.test/src/test/resources/TestData.xlsx
+++ b/com.pathnxt.test/src/test/resources/TestData.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="4275" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="4275" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="irctc" sheetId="1" r:id="rId1"/>
     <sheet name="redbus" sheetId="2" r:id="rId2"/>
     <sheet name="window" sheetId="3" r:id="rId3"/>
     <sheet name="tab" sheetId="4" r:id="rId4"/>
+    <sheet name="upload" sheetId="5" r:id="rId5"/>
+    <sheet name="download" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I12"/>
+  <oleSize ref="A1:P12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>from</t>
   </si>
@@ -117,6 +119,24 @@
   </si>
   <si>
     <t>Hello!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">file url </t>
+  </si>
+  <si>
+    <t>url4</t>
+  </si>
+  <si>
+    <t>file path</t>
+  </si>
+  <si>
+    <t>C:\Users\-hp-\Desktop\index.png</t>
+  </si>
+  <si>
+    <t>file url</t>
+  </si>
+  <si>
+    <t>url5</t>
   </si>
 </sst>
 </file>
@@ -625,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -695,4 +715,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added two new test scripts along with pom classes
</commit_message>
<xml_diff>
--- a/com.pathnxt.test/src/test/resources/TestData.xlsx
+++ b/com.pathnxt.test/src/test/resources/TestData.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="2" windowHeight="4500" windowWidth="16545" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="4500"/>
   </bookViews>
   <sheets>
-    <sheet name="irctc" r:id="rId1" sheetId="1"/>
-    <sheet name="redbus" r:id="rId2" sheetId="2"/>
-    <sheet name="window" r:id="rId3" sheetId="3"/>
-    <sheet name="tab" r:id="rId4" sheetId="4"/>
-    <sheet name="upload" r:id="rId5" sheetId="5"/>
-    <sheet name="download" r:id="rId6" sheetId="6"/>
-    <sheet name="table" r:id="rId7" sheetId="7"/>
-    <sheet name="calender" r:id="rId8" sheetId="8"/>
-    <sheet name="dropdown" r:id="rId9" sheetId="9"/>
+    <sheet name="irctc" sheetId="1" r:id="rId1"/>
+    <sheet name="redbus" sheetId="2" r:id="rId2"/>
+    <sheet name="window" sheetId="3" r:id="rId3"/>
+    <sheet name="tab" sheetId="4" r:id="rId4"/>
+    <sheet name="upload" sheetId="5" r:id="rId5"/>
+    <sheet name="download" sheetId="6" r:id="rId6"/>
+    <sheet name="table" sheetId="7" r:id="rId7"/>
+    <sheet name="calender" sheetId="8" r:id="rId8"/>
+    <sheet name="dropdown" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P12"/>
+  <oleSize ref="A1:P13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>from</t>
   </si>
@@ -151,23 +151,13 @@
     <t>Javascript</t>
   </si>
   <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Dot Net</t>
-  </si>
-  <si>
-    <t>Python</t>
+    <t>train number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,17 +191,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -228,10 +218,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -266,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,7 +291,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,7 +379,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -398,13 +388,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -414,7 +404,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -423,7 +413,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -432,7 +422,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -442,12 +432,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -478,7 +468,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -497,7 +487,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -509,20 +499,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,8 +529,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -552,15 +546,18 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2">
+        <v>12284</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -568,7 +565,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,13 +588,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -605,12 +602,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,13 +659,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -676,12 +673,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,13 +735,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -752,7 +749,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,13 +769,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -797,13 +794,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -828,14 +825,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -854,21 +851,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -891,6 +888,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Restassured components in the framework
</commit_message>
<xml_diff>
--- a/com.pathnxt.test/src/test/resources/TestData.xlsx
+++ b/com.pathnxt.test/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="4500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="4500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="irctc" sheetId="1" r:id="rId1"/>
@@ -12,19 +12,20 @@
     <sheet name="redbus" sheetId="2" r:id="rId3"/>
     <sheet name="window" sheetId="3" r:id="rId4"/>
     <sheet name="tab" sheetId="4" r:id="rId5"/>
-    <sheet name="upload" sheetId="5" r:id="rId6"/>
-    <sheet name="download" sheetId="6" r:id="rId7"/>
-    <sheet name="table" sheetId="7" r:id="rId8"/>
-    <sheet name="calender" sheetId="8" r:id="rId9"/>
-    <sheet name="dropdown" sheetId="9" r:id="rId10"/>
+    <sheet name="restassured" sheetId="11" r:id="rId6"/>
+    <sheet name="upload" sheetId="5" r:id="rId7"/>
+    <sheet name="download" sheetId="6" r:id="rId8"/>
+    <sheet name="table" sheetId="7" r:id="rId9"/>
+    <sheet name="calender" sheetId="8" r:id="rId10"/>
+    <sheet name="dropdown" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I13"/>
+  <oleSize ref="A1:P13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>from</t>
   </si>
@@ -198,6 +199,27 @@
   </si>
   <si>
     <t>https://the-internet.herokuapp.com/secure</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>engineer</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>rakesh</t>
+  </si>
+  <si>
+    <t>actor</t>
   </si>
 </sst>
 </file>
@@ -615,6 +637,31 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -867,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -941,6 +988,61 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -973,7 +1075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -998,7 +1100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1028,29 +1130,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>